<commit_message>
🔄 Mise à jour du fichier Excel public
</commit_message>
<xml_diff>
--- a/docs/epexspot_prices.xlsx
+++ b/docs/epexspot_prices.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EI25"/>
+  <dimension ref="A1:EJ25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1131,6 +1131,11 @@
           <t>30-oct.</t>
         </is>
       </c>
+      <c r="EJ1" s="1" t="inlineStr">
+        <is>
+          <t>31-oct.</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1570,6 +1575,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2009,6 +2019,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2448,6 +2463,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2887,6 +2907,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -3326,6 +3351,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -3765,6 +3795,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -4204,6 +4239,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -4643,6 +4683,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -5082,6 +5127,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -5521,6 +5571,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -5960,6 +6015,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -6399,6 +6459,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -6838,6 +6903,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -7277,6 +7347,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -7716,6 +7791,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -8155,6 +8235,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -8594,6 +8679,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -9033,6 +9123,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -9472,6 +9567,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -9911,6 +10011,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -10350,6 +10455,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -10789,6 +10899,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -11228,6 +11343,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="EJ24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -11663,6 +11783,11 @@
         <v>76.01000000000001</v>
       </c>
       <c r="EI25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="EJ25" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -11679,7 +11804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13047,6 +13172,16 @@
       </c>
       <c r="B136" t="n">
         <v>30.5</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>30.6</v>
       </c>
     </row>
   </sheetData>
@@ -13060,7 +13195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14414,6 +14549,16 @@
         <v>78.06</v>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>78.56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>